<commit_message>
Made some minor changes and edits.
</commit_message>
<xml_diff>
--- a/Twitter Regex.xlsx
+++ b/Twitter Regex.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanspangler/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanspangler/StabilityProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -548,9 +548,6 @@
     <t>([^.?!]*)(\b(homeless)\b)([^.?!]*)</t>
   </si>
   <si>
-    <t>([^.?!]*)(\b(slum)\b)([^.?!]*)</t>
-  </si>
-  <si>
     <t>([^.?!]*)(\b(incompetence)\b)([^.?!]*)</t>
   </si>
   <si>
@@ -920,9 +917,6 @@
     <t>([^.?!]*)(\b((human)|(basic)|(civil))\b)([^.?!]*)(rights)</t>
   </si>
   <si>
-    <t>([^.?!]*)(\b(rights)\b)([^.?!]*)((human)|(basic)|(civil))</t>
-  </si>
-  <si>
     <t>([^.?!]*)(\b((white)|(far right))\b)([^.?!]*)(nationalists?)</t>
   </si>
   <si>
@@ -1380,6 +1374,12 @@
   </si>
   <si>
     <t>([^.?!]*)(\b(police)\b)([^.?!]*)((hate)|(fuck(ing)?)|(brutality)|(corrupt(ion)?))</t>
+  </si>
+  <si>
+    <t>([^.?!]*)(\b(slums?)\b)([^.?!]*)</t>
+  </si>
+  <si>
+    <t>([^.?!]*)(\b(rights?)\b)([^.?!]*)((human)|(basic)|(civil))</t>
   </si>
 </sst>
 </file>
@@ -1700,8 +1700,8 @@
   <dimension ref="A1:F450"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D446" sqref="D446"/>
+      <pane ySplit="1" topLeftCell="A438" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A452" sqref="A452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1718,13 +1718,13 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F1" t="s">
         <v>104</v>
@@ -3360,7 +3360,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -3374,7 +3374,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -3518,7 +3518,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -3535,7 +3535,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -3552,7 +3552,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B111">
         <v>1</v>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -3583,7 +3583,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C113">
         <v>1</v>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -3611,7 +3611,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C115">
         <v>1</v>
@@ -3625,7 +3625,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -3639,7 +3639,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -3653,7 +3653,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -3667,7 +3667,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -3681,7 +3681,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -3695,7 +3695,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C121">
         <v>1</v>
@@ -3709,7 +3709,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -3720,7 +3720,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -3734,7 +3734,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C124">
         <v>1</v>
@@ -3748,7 +3748,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C125">
         <v>1</v>
@@ -3762,7 +3762,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C126">
         <v>1</v>
@@ -3776,7 +3776,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -3790,7 +3790,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C128">
         <v>1</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C130">
         <v>1</v>
@@ -3832,7 +3832,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C131">
         <v>1</v>
@@ -3846,7 +3846,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C132">
         <v>1</v>
@@ -3860,7 +3860,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -3874,7 +3874,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C134">
         <v>1</v>
@@ -3888,7 +3888,7 @@
     </row>
     <row r="135" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -3902,7 +3902,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -3916,7 +3916,7 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -3930,7 +3930,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -3944,7 +3944,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -3958,7 +3958,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -3972,7 +3972,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -3997,7 +3997,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -4008,7 +4008,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -4019,7 +4019,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -4030,7 +4030,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C147">
         <v>1</v>
@@ -4052,7 +4052,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C148">
         <v>1</v>
@@ -4063,7 +4063,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C149">
         <v>1</v>
@@ -4074,7 +4074,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C150">
         <v>1</v>
@@ -4085,7 +4085,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C151">
         <v>1</v>
@@ -4096,7 +4096,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C152">
         <v>1</v>
@@ -4107,7 +4107,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -4118,7 +4118,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -4129,7 +4129,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C155">
         <v>1</v>
@@ -4140,7 +4140,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C156">
         <v>1</v>
@@ -4151,7 +4151,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C157">
         <v>1</v>
@@ -4162,7 +4162,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -4173,7 +4173,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -4184,227 +4184,248 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>205</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>241</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>423</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>199</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>242</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>206</v>
       </c>
-      <c r="C160">
-        <v>1</v>
-      </c>
-      <c r="D160">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>242</v>
-      </c>
-      <c r="C161">
-        <v>1</v>
-      </c>
-      <c r="D161">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>425</v>
-      </c>
-      <c r="C162">
-        <v>1</v>
-      </c>
-      <c r="D162">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>200</v>
-      </c>
-      <c r="C163">
-        <v>1</v>
-      </c>
-      <c r="D163">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>243</v>
-      </c>
-      <c r="C164">
-        <v>1</v>
-      </c>
-      <c r="D164">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
+      <c r="C165">
+        <v>1</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
         <v>207</v>
       </c>
-      <c r="C165">
-        <v>1</v>
-      </c>
-      <c r="D165">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
+      <c r="C166">
+        <v>1</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>208</v>
       </c>
-      <c r="C166">
-        <v>1</v>
-      </c>
-      <c r="D166">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>209</v>
       </c>
-      <c r="C167">
-        <v>1</v>
-      </c>
-      <c r="D167">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
+      <c r="C168">
+        <v>1</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>210</v>
       </c>
-      <c r="C168">
-        <v>1</v>
-      </c>
-      <c r="D168">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
         <v>211</v>
       </c>
-      <c r="C169">
-        <v>1</v>
-      </c>
-      <c r="D169">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
+      <c r="C170">
+        <v>1</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
         <v>212</v>
       </c>
-      <c r="C170">
-        <v>1</v>
-      </c>
-      <c r="D170">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
+      <c r="C171">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
         <v>213</v>
       </c>
-      <c r="C171">
-        <v>1</v>
-      </c>
-      <c r="D171">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
         <v>214</v>
       </c>
-      <c r="C172">
-        <v>1</v>
-      </c>
-      <c r="D172">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
+      <c r="C173">
+        <v>1</v>
+      </c>
+      <c r="D173">
+        <v>1</v>
+      </c>
+      <c r="F173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
         <v>215</v>
       </c>
-      <c r="C173">
-        <v>1</v>
-      </c>
-      <c r="D173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
+      <c r="C174">
+        <v>1</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="F174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
         <v>216</v>
       </c>
-      <c r="C174">
-        <v>1</v>
-      </c>
-      <c r="D174">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
+      <c r="C175">
+        <v>1</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+      <c r="F175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
         <v>217</v>
       </c>
-      <c r="C175">
-        <v>1</v>
-      </c>
-      <c r="D175">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
-        <v>218</v>
-      </c>
       <c r="C176">
         <v>1</v>
       </c>
       <c r="D176">
+        <v>1</v>
+      </c>
+      <c r="F176">
         <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C177">
         <v>1</v>
       </c>
       <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="F177">
         <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C178">
         <v>1</v>
       </c>
       <c r="D178">
+        <v>1</v>
+      </c>
+      <c r="F178">
         <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C179">
         <v>1</v>
       </c>
       <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="F179">
         <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -4418,7 +4439,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C181">
         <v>1</v>
@@ -4432,7 +4453,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C182">
         <v>1</v>
@@ -4446,7 +4467,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C183">
         <v>1</v>
@@ -4457,7 +4478,7 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C184">
         <v>1</v>
@@ -4471,7 +4492,7 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C185">
         <v>1</v>
@@ -4485,7 +4506,7 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C186">
         <v>1</v>
@@ -4499,7 +4520,7 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C187">
         <v>1</v>
@@ -4513,7 +4534,7 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C188">
         <v>1</v>
@@ -4527,7 +4548,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C189">
         <v>1</v>
@@ -4541,7 +4562,7 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C190">
         <v>1</v>
@@ -4678,7 +4699,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B200">
         <v>2</v>
@@ -4692,7 +4713,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B201">
         <v>2</v>
@@ -4706,7 +4727,7 @@
     </row>
     <row r="202" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B202">
         <v>2</v>
@@ -4762,7 +4783,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B206">
         <v>3</v>
@@ -4776,7 +4797,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B207">
         <v>3</v>
@@ -4790,7 +4811,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B208">
         <v>3</v>
@@ -4804,7 +4825,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B209">
         <v>3</v>
@@ -4818,7 +4839,7 @@
     </row>
     <row r="210" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B210">
         <v>3</v>
@@ -4832,7 +4853,7 @@
     </row>
     <row r="211" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B211">
         <v>3</v>
@@ -4888,7 +4909,7 @@
     </row>
     <row r="215" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B215">
         <v>4</v>
@@ -4902,7 +4923,7 @@
     </row>
     <row r="216" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B216">
         <v>4</v>
@@ -4930,7 +4951,7 @@
     </row>
     <row r="218" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B218">
         <v>5</v>
@@ -4944,7 +4965,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B219">
         <v>1</v>
@@ -4958,7 +4979,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B220">
         <v>1</v>
@@ -4972,7 +4993,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B221">
         <v>1</v>
@@ -4986,7 +5007,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B222">
         <v>1</v>
@@ -5000,7 +5021,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B223">
         <v>1</v>
@@ -5014,7 +5035,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B224">
         <v>1</v>
@@ -5028,7 +5049,7 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B225">
         <v>1</v>
@@ -5042,7 +5063,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B226">
         <v>1</v>
@@ -5056,7 +5077,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -5073,7 +5094,7 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B228">
         <v>1</v>
@@ -5090,7 +5111,7 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C229">
         <v>6</v>
@@ -5104,7 +5125,7 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C230">
         <v>6</v>
@@ -5118,7 +5139,7 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C231">
         <v>6</v>
@@ -5132,7 +5153,7 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C232">
         <v>6</v>
@@ -5146,7 +5167,7 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C233">
         <v>6</v>
@@ -5160,7 +5181,7 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C234">
         <v>6</v>
@@ -5174,7 +5195,7 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C235">
         <v>6</v>
@@ -5188,7 +5209,7 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C236">
         <v>6</v>
@@ -5202,7 +5223,7 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C237">
         <v>6</v>
@@ -5216,7 +5237,7 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C238">
         <v>6</v>
@@ -5230,7 +5251,7 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C239">
         <v>6</v>
@@ -5244,7 +5265,7 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C240">
         <v>6</v>
@@ -5258,7 +5279,7 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C241">
         <v>6</v>
@@ -5272,7 +5293,7 @@
     </row>
     <row r="242" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B242">
         <v>1</v>
@@ -5342,7 +5363,7 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B247">
         <v>1</v>
@@ -5356,7 +5377,7 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C248">
         <v>6</v>
@@ -5367,7 +5388,7 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B249">
         <v>2</v>
@@ -5381,7 +5402,7 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B250">
         <v>2</v>
@@ -5395,7 +5416,7 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B251">
         <v>2</v>
@@ -5409,7 +5430,7 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B252">
         <v>2</v>
@@ -5423,7 +5444,7 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B253">
         <v>2</v>
@@ -5512,7 +5533,7 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B260">
         <v>3</v>
@@ -5523,7 +5544,7 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B261">
         <v>3</v>
@@ -5537,7 +5558,7 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B262">
         <v>3</v>
@@ -5582,7 +5603,7 @@
     </row>
     <row r="265" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B265">
         <v>5</v>
@@ -5599,7 +5620,7 @@
     </row>
     <row r="266" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B266">
         <v>5</v>
@@ -5610,7 +5631,7 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B267">
         <v>1</v>
@@ -5621,7 +5642,7 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B268">
         <v>1</v>
@@ -5632,7 +5653,7 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B269">
         <v>1</v>
@@ -5643,7 +5664,7 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B270">
         <v>1</v>
@@ -5654,7 +5675,7 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B271">
         <v>1</v>
@@ -5665,7 +5686,7 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B272">
         <v>1</v>
@@ -5676,7 +5697,7 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B273">
         <v>1</v>
@@ -5687,7 +5708,7 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B274">
         <v>1</v>
@@ -5698,7 +5719,7 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B275">
         <v>1</v>
@@ -5709,7 +5730,7 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B276">
         <v>1</v>
@@ -5720,7 +5741,7 @@
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B277">
         <v>1</v>
@@ -5787,7 +5808,7 @@
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B282">
         <v>1</v>
@@ -5798,7 +5819,7 @@
     </row>
     <row r="283" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B283">
         <v>1</v>
@@ -5809,7 +5830,7 @@
     </row>
     <row r="284" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B284">
         <v>1</v>
@@ -5820,7 +5841,7 @@
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B285">
         <v>1</v>
@@ -5834,7 +5855,7 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B286">
         <v>1</v>
@@ -5862,7 +5883,7 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B288">
         <v>1</v>
@@ -5876,7 +5897,7 @@
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
-        <v>173</v>
+        <v>449</v>
       </c>
       <c r="B289">
         <v>1</v>
@@ -5887,7 +5908,7 @@
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B290">
         <v>1</v>
@@ -5901,7 +5922,7 @@
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B291">
         <v>1</v>
@@ -5915,7 +5936,7 @@
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B292">
         <v>1</v>
@@ -5929,7 +5950,7 @@
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B293">
         <v>1</v>
@@ -5940,7 +5961,7 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B294">
         <v>1</v>
@@ -5951,7 +5972,7 @@
     </row>
     <row r="295" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B295">
         <v>1</v>
@@ -5962,7 +5983,7 @@
     </row>
     <row r="296" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B296">
         <v>1</v>
@@ -5973,7 +5994,7 @@
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B297">
         <v>1</v>
@@ -5984,7 +6005,7 @@
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B298">
         <v>1</v>
@@ -5995,7 +6016,7 @@
     </row>
     <row r="299" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B299">
         <v>1</v>
@@ -6006,7 +6027,7 @@
     </row>
     <row r="300" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B300">
         <v>1</v>
@@ -6017,7 +6038,7 @@
     </row>
     <row r="301" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B301">
         <v>1</v>
@@ -6028,7 +6049,7 @@
     </row>
     <row r="302" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B302">
         <v>1</v>
@@ -6039,7 +6060,7 @@
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B303">
         <v>1</v>
@@ -6050,7 +6071,7 @@
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B304">
         <v>1</v>
@@ -6061,7 +6082,7 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B305">
         <v>1</v>
@@ -6072,7 +6093,7 @@
     </row>
     <row r="306" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B306">
         <v>1</v>
@@ -6083,7 +6104,7 @@
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B307">
         <v>1</v>
@@ -6094,7 +6115,7 @@
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B308">
         <v>1</v>
@@ -6105,7 +6126,7 @@
     </row>
     <row r="309" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C309">
         <v>11</v>
@@ -6116,7 +6137,7 @@
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C310">
         <v>11</v>
@@ -6127,7 +6148,7 @@
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C311">
         <v>11</v>
@@ -6138,7 +6159,7 @@
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C312">
         <v>11</v>
@@ -6226,7 +6247,7 @@
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C320">
         <v>11</v>
@@ -6369,7 +6390,7 @@
     </row>
     <row r="333" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C333">
         <v>11</v>
@@ -6380,7 +6401,7 @@
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C334">
         <v>11</v>
@@ -6402,7 +6423,7 @@
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C336">
         <v>11</v>
@@ -6413,7 +6434,7 @@
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C337">
         <v>11</v>
@@ -6545,7 +6566,7 @@
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C349">
         <v>11</v>
@@ -6622,7 +6643,7 @@
     </row>
     <row r="356" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C356">
         <v>11</v>
@@ -6633,7 +6654,7 @@
     </row>
     <row r="357" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A357" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B357">
         <v>2</v>
@@ -6644,7 +6665,7 @@
     </row>
     <row r="358" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A358" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B358">
         <v>2</v>
@@ -6655,7 +6676,7 @@
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A359" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B359">
         <v>2</v>
@@ -6666,7 +6687,7 @@
     </row>
     <row r="360" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A360" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B360">
         <v>2</v>
@@ -6677,7 +6698,7 @@
     </row>
     <row r="361" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A361" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B361">
         <v>2</v>
@@ -6688,7 +6709,7 @@
     </row>
     <row r="362" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A362" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B362">
         <v>2</v>
@@ -6699,7 +6720,7 @@
     </row>
     <row r="363" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A363" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B363">
         <v>2</v>
@@ -6710,7 +6731,7 @@
     </row>
     <row r="364" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A364" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B364">
         <v>2</v>
@@ -6721,7 +6742,7 @@
     </row>
     <row r="365" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A365" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B365">
         <v>2</v>
@@ -6732,7 +6753,7 @@
     </row>
     <row r="366" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A366" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B366">
         <v>2</v>
@@ -6743,7 +6764,7 @@
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A367" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B367">
         <v>2</v>
@@ -6754,7 +6775,7 @@
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A368" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B368">
         <v>2</v>
@@ -6765,7 +6786,7 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B369">
         <v>2</v>
@@ -6776,7 +6797,7 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B370">
         <v>2</v>
@@ -6787,7 +6808,7 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B371">
         <v>2</v>
@@ -6798,7 +6819,7 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B372">
         <v>2</v>
@@ -6809,7 +6830,7 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B373">
         <v>2</v>
@@ -6820,7 +6841,7 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B374">
         <v>2</v>
@@ -6831,7 +6852,7 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B375">
         <v>2</v>
@@ -6842,7 +6863,7 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B376">
         <v>2</v>
@@ -6853,7 +6874,7 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B377">
         <v>2</v>
@@ -6864,7 +6885,7 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B378">
         <v>2</v>
@@ -6875,7 +6896,7 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B379">
         <v>2</v>
@@ -6886,7 +6907,7 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B380">
         <v>2</v>
@@ -6897,7 +6918,7 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B381">
         <v>2</v>
@@ -6908,7 +6929,7 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B382">
         <v>2</v>
@@ -6919,7 +6940,7 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B383">
         <v>2</v>
@@ -6930,7 +6951,7 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B384">
         <v>2</v>
@@ -6955,7 +6976,7 @@
     </row>
     <row r="386" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A386" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B386">
         <v>2</v>
@@ -6966,7 +6987,7 @@
     </row>
     <row r="387" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A387" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B387">
         <v>2</v>
@@ -6977,7 +6998,7 @@
     </row>
     <row r="388" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A388" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B388">
         <v>2</v>
@@ -6988,7 +7009,7 @@
     </row>
     <row r="389" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A389" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B389">
         <v>2</v>
@@ -6999,7 +7020,7 @@
     </row>
     <row r="390" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A390" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B390">
         <v>2</v>
@@ -7010,7 +7031,7 @@
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A391" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B391">
         <v>2</v>
@@ -7021,7 +7042,7 @@
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A392" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B392">
         <v>2</v>
@@ -7032,7 +7053,7 @@
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A393" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B393">
         <v>2</v>
@@ -7043,7 +7064,7 @@
     </row>
     <row r="394" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A394" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B394">
         <v>2</v>
@@ -7054,7 +7075,7 @@
     </row>
     <row r="395" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A395" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B395">
         <v>2</v>
@@ -7065,7 +7086,7 @@
     </row>
     <row r="396" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B396">
         <v>2</v>
@@ -7076,7 +7097,7 @@
     </row>
     <row r="397" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A397" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B397">
         <v>2</v>
@@ -7087,7 +7108,7 @@
     </row>
     <row r="398" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A398" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B398">
         <v>2</v>
@@ -7098,7 +7119,7 @@
     </row>
     <row r="399" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A399" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B399">
         <v>2</v>
@@ -7109,7 +7130,7 @@
     </row>
     <row r="400" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A400" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B400">
         <v>2</v>
@@ -7120,7 +7141,7 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B401">
         <v>3</v>
@@ -7131,7 +7152,7 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B402">
         <v>3</v>
@@ -7142,7 +7163,7 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B403">
         <v>3</v>
@@ -7153,7 +7174,7 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B404">
         <v>3</v>
@@ -7164,7 +7185,7 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B405">
         <v>3</v>
@@ -7175,7 +7196,7 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B406">
         <v>3</v>
@@ -7186,7 +7207,7 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B407">
         <v>3</v>
@@ -7197,7 +7218,7 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B408">
         <v>3</v>
@@ -7208,7 +7229,7 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A409" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B409">
         <v>3</v>
@@ -7219,7 +7240,7 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A410" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B410">
         <v>3</v>
@@ -7230,7 +7251,7 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A411" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B411">
         <v>3</v>
@@ -7241,7 +7262,7 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A412" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B412">
         <v>3</v>
@@ -7252,7 +7273,7 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B413">
         <v>3</v>
@@ -7263,7 +7284,7 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B414">
         <v>3</v>
@@ -7274,7 +7295,7 @@
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B415">
         <v>3</v>
@@ -7285,7 +7306,7 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B416">
         <v>3</v>
@@ -7296,7 +7317,7 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417" s="1" t="s">
-        <v>297</v>
+        <v>450</v>
       </c>
       <c r="B417">
         <v>3</v>
@@ -7307,7 +7328,7 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B418">
         <v>3</v>
@@ -7318,7 +7339,7 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B419">
         <v>3</v>
@@ -7329,7 +7350,7 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B420">
         <v>3</v>
@@ -7340,7 +7361,7 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B421">
         <v>3</v>
@@ -7351,7 +7372,7 @@
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B422">
         <v>3</v>
@@ -7362,7 +7383,7 @@
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B423">
         <v>3</v>
@@ -7373,7 +7394,7 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B424">
         <v>3</v>
@@ -7384,7 +7405,7 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B425">
         <v>3</v>
@@ -7395,7 +7416,7 @@
     </row>
     <row r="426" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A426" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B426">
         <v>3</v>
@@ -7406,7 +7427,7 @@
     </row>
     <row r="427" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A427" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B427">
         <v>3</v>
@@ -7417,7 +7438,7 @@
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B428">
         <v>3</v>
@@ -7428,7 +7449,7 @@
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B429">
         <v>3</v>
@@ -7439,7 +7460,7 @@
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B430">
         <v>4</v>
@@ -7450,7 +7471,7 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B431">
         <v>4</v>
@@ -7461,7 +7482,7 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A432" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B432">
         <v>4</v>
@@ -7472,7 +7493,7 @@
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A433" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B433">
         <v>4</v>
@@ -7483,7 +7504,7 @@
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A434" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B434">
         <v>4</v>
@@ -7494,7 +7515,7 @@
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A435" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B435">
         <v>4</v>
@@ -7505,7 +7526,7 @@
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A436" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B436">
         <v>4</v>
@@ -7516,7 +7537,7 @@
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A437" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B437">
         <v>4</v>
@@ -7527,7 +7548,7 @@
     </row>
     <row r="438" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A438" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B438">
         <v>4</v>
@@ -7538,7 +7559,7 @@
     </row>
     <row r="439" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A439" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B439">
         <v>4</v>
@@ -7549,7 +7570,7 @@
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A440" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B440">
         <v>4</v>
@@ -7560,7 +7581,7 @@
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A441" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B441">
         <v>4</v>
@@ -7571,7 +7592,7 @@
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A442" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B442">
         <v>5</v>
@@ -7582,7 +7603,7 @@
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A443" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B443">
         <v>5</v>
@@ -7593,7 +7614,7 @@
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A444" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B444">
         <v>5</v>
@@ -7604,7 +7625,7 @@
     </row>
     <row r="445" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A445" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B445">
         <v>5</v>
@@ -7615,7 +7636,7 @@
     </row>
     <row r="446" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A446" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B446">
         <v>5</v>
@@ -7626,7 +7647,7 @@
     </row>
     <row r="447" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A447" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B447">
         <v>5</v>
@@ -7637,7 +7658,7 @@
     </row>
     <row r="448" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A448" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B448">
         <v>5</v>
@@ -7648,7 +7669,7 @@
     </row>
     <row r="449" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A449" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B449">
         <v>5</v>
@@ -7659,7 +7680,7 @@
     </row>
     <row r="450" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A450" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B450">
         <v>5</v>

</xml_diff>